<commit_message>
Updated to version 1.0.1
Added new algorithm RPCA-SPGL1
</commit_message>
<xml_diff>
--- a/algorithms.xlsx
+++ b/algorithms.xlsx
@@ -5,16 +5,15 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\alrslibrary\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\lrslibrary\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="10320" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="10320" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Algs" sheetId="1" r:id="rId1"/>
-    <sheet name="Speed" sheetId="2" r:id="rId2"/>
-    <sheet name="Speed (Rank)" sheetId="3" r:id="rId3"/>
+    <sheet name="CPU" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -68,43 +67,6 @@
     <author>asobra01</author>
   </authors>
   <commentList>
-    <comment ref="E1" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>asobra01:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Time to decompose:
-2304x51 Matrix
-or
-48x48x51 Tensor</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>asobra01</author>
-  </authors>
-  <commentList>
     <comment ref="F1" authorId="0" shapeId="0">
       <text>
         <r>
@@ -137,7 +99,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="720" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="201">
   <si>
     <t>Method</t>
   </si>
@@ -731,6 +693,15 @@
   </si>
   <si>
     <t>Semi Non-negative Matrix Factorization</t>
+  </si>
+  <si>
+    <t>SPGL1</t>
+  </si>
+  <si>
+    <t>A variational approach to SPCP (Aravkin et al. 2014)</t>
+  </si>
+  <si>
+    <t>16.60</t>
   </si>
 </sst>
 </file>
@@ -841,7 +812,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -882,21 +853,6 @@
     </xf>
     <xf numFmtId="2" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1213,7 +1169,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E65"/>
+  <dimension ref="A1:E66"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
@@ -1243,13 +1199,13 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="s">
-        <v>126</v>
-      </c>
-      <c r="B2" s="22" t="s">
+      <c r="A2" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="B2" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="C2" s="21" t="s">
+      <c r="C2" s="16" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="3">
@@ -1260,13 +1216,13 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="21" t="s">
-        <v>126</v>
-      </c>
-      <c r="B3" s="21" t="s">
+      <c r="A3" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="B3" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="C3" s="21" t="s">
+      <c r="C3" s="16" t="s">
         <v>5</v>
       </c>
       <c r="D3" s="5">
@@ -1277,13 +1233,13 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="21" t="s">
-        <v>126</v>
-      </c>
-      <c r="B4" s="21" t="s">
+      <c r="A4" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="B4" s="16" t="s">
         <v>192</v>
       </c>
-      <c r="C4" s="21" t="s">
+      <c r="C4" s="16" t="s">
         <v>193</v>
       </c>
       <c r="D4" s="5">
@@ -1294,13 +1250,13 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="21" t="s">
-        <v>126</v>
-      </c>
-      <c r="B5" s="21" t="s">
+      <c r="A5" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="B5" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="C5" s="21" t="s">
+      <c r="C5" s="16" t="s">
         <v>6</v>
       </c>
       <c r="D5" s="5">
@@ -1311,13 +1267,13 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="21" t="s">
-        <v>126</v>
-      </c>
-      <c r="B6" s="21" t="s">
+      <c r="A6" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="B6" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="C6" s="21" t="s">
+      <c r="C6" s="16" t="s">
         <v>7</v>
       </c>
       <c r="D6" s="11">
@@ -1328,13 +1284,13 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="21" t="s">
-        <v>126</v>
-      </c>
-      <c r="B7" s="21" t="s">
+      <c r="A7" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="B7" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="C7" s="21" t="s">
+      <c r="C7" s="16" t="s">
         <v>8</v>
       </c>
       <c r="D7" s="3">
@@ -1345,13 +1301,13 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="21" t="s">
-        <v>126</v>
-      </c>
-      <c r="B8" s="21" t="s">
+      <c r="A8" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="B8" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="C8" s="21" t="s">
+      <c r="C8" s="16" t="s">
         <v>9</v>
       </c>
       <c r="D8" s="5">
@@ -1362,13 +1318,13 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="21" t="s">
-        <v>126</v>
-      </c>
-      <c r="B9" s="21" t="s">
+      <c r="A9" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="B9" s="16" t="s">
         <v>133</v>
       </c>
-      <c r="C9" s="21" t="s">
+      <c r="C9" s="16" t="s">
         <v>10</v>
       </c>
       <c r="D9" s="5">
@@ -1379,13 +1335,13 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="21" t="s">
-        <v>126</v>
-      </c>
-      <c r="B10" s="21" t="s">
+      <c r="A10" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="B10" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="C10" s="21" t="s">
+      <c r="C10" s="16" t="s">
         <v>11</v>
       </c>
       <c r="D10" s="3">
@@ -1396,13 +1352,13 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="21" t="s">
-        <v>126</v>
-      </c>
-      <c r="B11" s="21" t="s">
+      <c r="A11" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="B11" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="C11" s="21" t="s">
+      <c r="C11" s="16" t="s">
         <v>12</v>
       </c>
       <c r="D11" s="5">
@@ -1413,13 +1369,13 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="21" t="s">
-        <v>126</v>
-      </c>
-      <c r="B12" s="21" t="s">
+      <c r="A12" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="B12" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="C12" s="21" t="s">
+      <c r="C12" s="16" t="s">
         <v>13</v>
       </c>
       <c r="D12" s="3">
@@ -1430,13 +1386,13 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="21" t="s">
-        <v>126</v>
-      </c>
-      <c r="B13" s="21" t="s">
+      <c r="A13" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="B13" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="C13" s="21" t="s">
+      <c r="C13" s="16" t="s">
         <v>14</v>
       </c>
       <c r="D13" s="7">
@@ -1447,13 +1403,13 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="21" t="s">
-        <v>126</v>
-      </c>
-      <c r="B14" s="21" t="s">
+      <c r="A14" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="B14" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="C14" s="21" t="s">
+      <c r="C14" s="16" t="s">
         <v>15</v>
       </c>
       <c r="D14" s="9">
@@ -1464,13 +1420,13 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="21" t="s">
-        <v>126</v>
-      </c>
-      <c r="B15" s="21" t="s">
+      <c r="A15" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="B15" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="C15" s="21" t="s">
+      <c r="C15" s="16" t="s">
         <v>16</v>
       </c>
       <c r="D15" s="3">
@@ -1481,13 +1437,13 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="21" t="s">
-        <v>126</v>
-      </c>
-      <c r="B16" s="21" t="s">
+      <c r="A16" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="B16" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="C16" s="21" t="s">
+      <c r="C16" s="16" t="s">
         <v>17</v>
       </c>
       <c r="D16" s="5">
@@ -1498,13 +1454,13 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="21" t="s">
-        <v>126</v>
-      </c>
-      <c r="B17" s="21" t="s">
+      <c r="A17" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="B17" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="C17" s="21" t="s">
+      <c r="C17" s="16" t="s">
         <v>18</v>
       </c>
       <c r="D17" s="5">
@@ -1515,13 +1471,13 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="21" t="s">
-        <v>126</v>
-      </c>
-      <c r="B18" s="21" t="s">
+      <c r="A18" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="B18" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="C18" s="21" t="s">
+      <c r="C18" s="16" t="s">
         <v>19</v>
       </c>
       <c r="D18" s="5">
@@ -1532,13 +1488,13 @@
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="21" t="s">
-        <v>126</v>
-      </c>
-      <c r="B19" s="21" t="s">
+      <c r="A19" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="B19" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="C19" s="21" t="s">
+      <c r="C19" s="16" t="s">
         <v>20</v>
       </c>
       <c r="D19" s="5">
@@ -1549,13 +1505,13 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="21" t="s">
-        <v>126</v>
-      </c>
-      <c r="B20" s="21" t="s">
+      <c r="A20" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="B20" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="C20" s="21" t="s">
+      <c r="C20" s="16" t="s">
         <v>21</v>
       </c>
       <c r="D20" s="5">
@@ -1566,13 +1522,13 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="21" t="s">
-        <v>126</v>
-      </c>
-      <c r="B21" s="21" t="s">
+      <c r="A21" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="B21" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="C21" s="21" t="s">
+      <c r="C21" s="16" t="s">
         <v>22</v>
       </c>
       <c r="D21" s="5">
@@ -1583,750 +1539,767 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="21" t="s">
-        <v>126</v>
-      </c>
-      <c r="B22" s="21" t="s">
+      <c r="A22" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="B22" s="16" t="s">
+        <v>198</v>
+      </c>
+      <c r="C22" s="16" t="s">
+        <v>199</v>
+      </c>
+      <c r="D22" s="11">
+        <v>3</v>
+      </c>
+      <c r="E22" s="12" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="B23" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="C22" s="21" t="s">
+      <c r="C23" s="16" t="s">
         <v>23</v>
-      </c>
-      <c r="D22" s="7">
-        <v>4</v>
-      </c>
-      <c r="E22" s="8" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="21" t="s">
-        <v>126</v>
-      </c>
-      <c r="B23" s="21" t="s">
-        <v>83</v>
-      </c>
-      <c r="C23" s="21" t="s">
-        <v>24</v>
       </c>
       <c r="D23" s="7">
         <v>4</v>
       </c>
       <c r="E23" s="8" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="B24" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="C24" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="D24" s="7">
+        <v>4</v>
+      </c>
+      <c r="E24" s="8" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="21" t="s">
-        <v>126</v>
-      </c>
-      <c r="B24" s="21" t="s">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="B25" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="C24" s="21" t="s">
+      <c r="C25" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="D24" s="3">
-        <v>2</v>
-      </c>
-      <c r="E24" s="4" t="s">
+      <c r="D25" s="3">
+        <v>2</v>
+      </c>
+      <c r="E25" s="4" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="21" t="s">
-        <v>126</v>
-      </c>
-      <c r="B25" s="21" t="s">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="B26" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="C25" s="21" t="s">
+      <c r="C26" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="D25" s="3">
-        <v>2</v>
-      </c>
-      <c r="E25" s="4" t="s">
+      <c r="D26" s="3">
+        <v>2</v>
+      </c>
+      <c r="E26" s="4" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="21" t="s">
-        <v>126</v>
-      </c>
-      <c r="B26" s="21" t="s">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="B27" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="C26" s="21" t="s">
+      <c r="C27" s="16" t="s">
         <v>27</v>
-      </c>
-      <c r="D26" s="7">
-        <v>4</v>
-      </c>
-      <c r="E26" s="8" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="21" t="s">
-        <v>126</v>
-      </c>
-      <c r="B27" s="21" t="s">
-        <v>87</v>
-      </c>
-      <c r="C27" s="21" t="s">
-        <v>28</v>
       </c>
       <c r="D27" s="7">
         <v>4</v>
       </c>
       <c r="E27" s="8" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="B28" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="C28" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="D28" s="7">
+        <v>4</v>
+      </c>
+      <c r="E28" s="8" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="21" t="s">
-        <v>126</v>
-      </c>
-      <c r="B28" s="21" t="s">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="B29" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="C28" s="21" t="s">
+      <c r="C29" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="D28" s="3">
-        <v>2</v>
-      </c>
-      <c r="E28" s="4" t="s">
+      <c r="D29" s="3">
+        <v>2</v>
+      </c>
+      <c r="E29" s="4" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="21" t="s">
-        <v>126</v>
-      </c>
-      <c r="B29" s="21" t="s">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="B30" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="C29" s="21" t="s">
+      <c r="C30" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="D29" s="3">
-        <v>2</v>
-      </c>
-      <c r="E29" s="4" t="s">
+      <c r="D30" s="3">
+        <v>2</v>
+      </c>
+      <c r="E30" s="4" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="21" t="s">
-        <v>126</v>
-      </c>
-      <c r="B30" s="21" t="s">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="B31" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="C30" s="21" t="s">
+      <c r="C31" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="D30" s="5">
-        <v>1</v>
-      </c>
-      <c r="E30" s="6" t="s">
+      <c r="D31" s="5">
+        <v>1</v>
+      </c>
+      <c r="E31" s="6" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="23" t="s">
-        <v>126</v>
-      </c>
-      <c r="B31" s="23" t="s">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="B32" s="18" t="s">
         <v>91</v>
       </c>
-      <c r="C31" s="23" t="s">
+      <c r="C32" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="D31" s="25">
-        <v>1</v>
-      </c>
-      <c r="E31" s="26" t="s">
+      <c r="D32" s="20">
+        <v>1</v>
+      </c>
+      <c r="E32" s="21" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="24" t="s">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="19" t="s">
         <v>127</v>
       </c>
-      <c r="B32" s="24" t="s">
+      <c r="B33" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="C32" s="24" t="s">
+      <c r="C33" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="D32" s="3">
-        <v>2</v>
-      </c>
-      <c r="E32" s="4" t="s">
+      <c r="D33" s="3">
+        <v>2</v>
+      </c>
+      <c r="E33" s="4" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="21" t="s">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="16" t="s">
         <v>127</v>
       </c>
-      <c r="B33" s="21" t="s">
+      <c r="B34" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="C33" s="21" t="s">
+      <c r="C34" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="D33" s="5">
-        <v>1</v>
-      </c>
-      <c r="E33" s="6" t="s">
+      <c r="D34" s="5">
+        <v>1</v>
+      </c>
+      <c r="E34" s="6" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="21" t="s">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="16" t="s">
         <v>127</v>
       </c>
-      <c r="B34" s="21" t="s">
+      <c r="B35" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="C34" s="21" t="s">
+      <c r="C35" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="D34" s="5">
-        <v>1</v>
-      </c>
-      <c r="E34" s="6" t="s">
+      <c r="D35" s="5">
+        <v>1</v>
+      </c>
+      <c r="E35" s="6" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="21" t="s">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="16" t="s">
         <v>127</v>
       </c>
-      <c r="B35" s="21" t="s">
+      <c r="B36" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="C35" s="21" t="s">
+      <c r="C36" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="D35" s="5">
-        <v>1</v>
-      </c>
-      <c r="E35" s="6" t="s">
+      <c r="D36" s="5">
+        <v>1</v>
+      </c>
+      <c r="E36" s="6" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="23" t="s">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="18" t="s">
         <v>127</v>
       </c>
-      <c r="B36" s="23" t="s">
+      <c r="B37" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="C36" s="23" t="s">
+      <c r="C37" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="D36" s="25">
-        <v>1</v>
-      </c>
-      <c r="E36" s="26" t="s">
+      <c r="D37" s="20">
+        <v>1</v>
+      </c>
+      <c r="E37" s="21" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="24" t="s">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="19" t="s">
         <v>128</v>
       </c>
-      <c r="B37" s="24" t="s">
+      <c r="B38" s="19" t="s">
         <v>97</v>
       </c>
-      <c r="C37" s="24" t="s">
+      <c r="C38" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="D37" s="5">
-        <v>1</v>
-      </c>
-      <c r="E37" s="6" t="s">
+      <c r="D38" s="5">
+        <v>1</v>
+      </c>
+      <c r="E38" s="6" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="21" t="s">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="16" t="s">
         <v>128</v>
       </c>
-      <c r="B38" s="21" t="s">
+      <c r="B39" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="C38" s="21" t="s">
+      <c r="C39" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="D38" s="5">
-        <v>1</v>
-      </c>
-      <c r="E38" s="6" t="s">
+      <c r="D39" s="5">
+        <v>1</v>
+      </c>
+      <c r="E39" s="6" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="21" t="s">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="16" t="s">
         <v>128</v>
       </c>
-      <c r="B39" s="21" t="s">
+      <c r="B40" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="C39" s="21" t="s">
+      <c r="C40" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="D39" s="5">
-        <v>1</v>
-      </c>
-      <c r="E39" s="6" t="s">
+      <c r="D40" s="5">
+        <v>1</v>
+      </c>
+      <c r="E40" s="6" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="21" t="s">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="16" t="s">
         <v>128</v>
       </c>
-      <c r="B40" s="21" t="s">
+      <c r="B41" s="16" t="s">
         <v>100</v>
       </c>
-      <c r="C40" s="21" t="s">
+      <c r="C41" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="D40" s="5">
-        <v>1</v>
-      </c>
-      <c r="E40" s="6" t="s">
+      <c r="D41" s="5">
+        <v>1</v>
+      </c>
+      <c r="E41" s="6" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="21" t="s">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="16" t="s">
         <v>128</v>
       </c>
-      <c r="B41" s="21" t="s">
+      <c r="B42" s="16" t="s">
         <v>101</v>
       </c>
-      <c r="C41" s="21" t="s">
+      <c r="C42" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="D41" s="3">
-        <v>2</v>
-      </c>
-      <c r="E41" s="4" t="s">
+      <c r="D42" s="3">
+        <v>2</v>
+      </c>
+      <c r="E42" s="4" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="21" t="s">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="16" t="s">
         <v>128</v>
       </c>
-      <c r="B42" s="21" t="s">
+      <c r="B43" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="C42" s="21" t="s">
+      <c r="C43" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="D42" s="5">
-        <v>1</v>
-      </c>
-      <c r="E42" s="6" t="s">
+      <c r="D43" s="5">
+        <v>1</v>
+      </c>
+      <c r="E43" s="6" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="21" t="s">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="16" t="s">
         <v>128</v>
       </c>
-      <c r="B43" s="21" t="s">
+      <c r="B44" s="16" t="s">
         <v>103</v>
       </c>
-      <c r="C43" s="21" t="s">
+      <c r="C44" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="D43" s="5">
-        <v>1</v>
-      </c>
-      <c r="E43" s="6" t="s">
+      <c r="D44" s="5">
+        <v>1</v>
+      </c>
+      <c r="E44" s="6" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="21" t="s">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="16" t="s">
         <v>128</v>
       </c>
-      <c r="B44" s="21" t="s">
+      <c r="B45" s="16" t="s">
         <v>104</v>
       </c>
-      <c r="C44" s="21" t="s">
+      <c r="C45" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="D44" s="5">
-        <v>1</v>
-      </c>
-      <c r="E44" s="6" t="s">
+      <c r="D45" s="5">
+        <v>1</v>
+      </c>
+      <c r="E45" s="6" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="21" t="s">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="16" t="s">
         <v>128</v>
       </c>
-      <c r="B45" s="21" t="s">
+      <c r="B46" s="16" t="s">
         <v>105</v>
       </c>
-      <c r="C45" s="21" t="s">
+      <c r="C46" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="D45" s="3">
-        <v>2</v>
-      </c>
-      <c r="E45" s="4" t="s">
+      <c r="D46" s="3">
+        <v>2</v>
+      </c>
+      <c r="E46" s="4" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="21" t="s">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="16" t="s">
         <v>128</v>
       </c>
-      <c r="B46" s="21" t="s">
+      <c r="B47" s="16" t="s">
         <v>106</v>
       </c>
-      <c r="C46" s="21" t="s">
+      <c r="C47" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="D46" s="3">
-        <v>2</v>
-      </c>
-      <c r="E46" s="4" t="s">
+      <c r="D47" s="3">
+        <v>2</v>
+      </c>
+      <c r="E47" s="4" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="21" t="s">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="16" t="s">
         <v>128</v>
       </c>
-      <c r="B47" s="21" t="s">
+      <c r="B48" s="16" t="s">
         <v>107</v>
       </c>
-      <c r="C47" s="21" t="s">
+      <c r="C48" s="16" t="s">
         <v>197</v>
       </c>
-      <c r="D47" s="5">
-        <v>1</v>
-      </c>
-      <c r="E47" s="6" t="s">
+      <c r="D48" s="5">
+        <v>1</v>
+      </c>
+      <c r="E48" s="6" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="23" t="s">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="18" t="s">
         <v>128</v>
       </c>
-      <c r="B48" s="23" t="s">
+      <c r="B49" s="18" t="s">
         <v>108</v>
       </c>
-      <c r="C48" s="23" t="s">
+      <c r="C49" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="D48" s="25">
-        <v>1</v>
-      </c>
-      <c r="E48" s="26" t="s">
+      <c r="D49" s="20">
+        <v>1</v>
+      </c>
+      <c r="E49" s="21" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="24" t="s">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="19" t="s">
         <v>129</v>
       </c>
-      <c r="B49" s="24" t="s">
+      <c r="B50" s="19" t="s">
         <v>109</v>
       </c>
-      <c r="C49" s="24" t="s">
+      <c r="C50" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="D49" s="3">
-        <v>2</v>
-      </c>
-      <c r="E49" s="4" t="s">
+      <c r="D50" s="3">
+        <v>2</v>
+      </c>
+      <c r="E50" s="4" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="21" t="s">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="16" t="s">
         <v>129</v>
       </c>
-      <c r="B50" s="21" t="s">
+      <c r="B51" s="16" t="s">
         <v>110</v>
       </c>
-      <c r="C50" s="21" t="s">
+      <c r="C51" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="D50" s="3">
-        <v>2</v>
-      </c>
-      <c r="E50" s="4" t="s">
+      <c r="D51" s="3">
+        <v>2</v>
+      </c>
+      <c r="E51" s="4" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="21" t="s">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="16" t="s">
         <v>129</v>
       </c>
-      <c r="B51" s="21" t="s">
+      <c r="B52" s="16" t="s">
         <v>111</v>
       </c>
-      <c r="C51" s="21" t="s">
+      <c r="C52" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="D51" s="5">
-        <v>1</v>
-      </c>
-      <c r="E51" s="6" t="s">
+      <c r="D52" s="5">
+        <v>1</v>
+      </c>
+      <c r="E52" s="6" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="21" t="s">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="16" t="s">
         <v>129</v>
       </c>
-      <c r="B52" s="21" t="s">
+      <c r="B53" s="16" t="s">
         <v>112</v>
       </c>
-      <c r="C52" s="21" t="s">
+      <c r="C53" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="D52" s="3">
-        <v>2</v>
-      </c>
-      <c r="E52" s="4" t="s">
+      <c r="D53" s="3">
+        <v>2</v>
+      </c>
+      <c r="E53" s="4" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="21" t="s">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="16" t="s">
         <v>129</v>
       </c>
-      <c r="B53" s="21" t="s">
+      <c r="B54" s="16" t="s">
         <v>113</v>
       </c>
-      <c r="C53" s="21" t="s">
+      <c r="C54" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="D53" s="3">
-        <v>2</v>
-      </c>
-      <c r="E53" s="4" t="s">
+      <c r="D54" s="3">
+        <v>2</v>
+      </c>
+      <c r="E54" s="4" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="23" t="s">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="B54" s="23" t="s">
+      <c r="B55" s="18" t="s">
         <v>114</v>
       </c>
-      <c r="C54" s="23" t="s">
+      <c r="C55" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="D54" s="27">
-        <v>2</v>
-      </c>
-      <c r="E54" s="28" t="s">
+      <c r="D55" s="22">
+        <v>2</v>
+      </c>
+      <c r="E55" s="23" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="24" t="s">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="19" t="s">
         <v>130</v>
       </c>
-      <c r="B55" s="24" t="s">
+      <c r="B56" s="19" t="s">
         <v>115</v>
       </c>
-      <c r="C55" s="24" t="s">
+      <c r="C56" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="D55" s="5">
-        <v>1</v>
-      </c>
-      <c r="E55" s="6" t="s">
+      <c r="D56" s="5">
+        <v>1</v>
+      </c>
+      <c r="E56" s="6" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="21" t="s">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" s="16" t="s">
         <v>130</v>
       </c>
-      <c r="B56" s="21" t="s">
+      <c r="B57" s="16" t="s">
         <v>116</v>
       </c>
-      <c r="C56" s="21" t="s">
+      <c r="C57" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="D56" s="3">
-        <v>2</v>
-      </c>
-      <c r="E56" s="4" t="s">
+      <c r="D57" s="3">
+        <v>2</v>
+      </c>
+      <c r="E57" s="4" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" s="21" t="s">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" s="16" t="s">
         <v>130</v>
       </c>
-      <c r="B57" s="21" t="s">
+      <c r="B58" s="16" t="s">
         <v>117</v>
       </c>
-      <c r="C57" s="21" t="s">
+      <c r="C58" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="D57" s="3">
-        <v>2</v>
-      </c>
-      <c r="E57" s="4" t="s">
+      <c r="D58" s="3">
+        <v>2</v>
+      </c>
+      <c r="E58" s="4" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" s="21" t="s">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" s="16" t="s">
         <v>130</v>
       </c>
-      <c r="B58" s="21" t="s">
+      <c r="B59" s="16" t="s">
         <v>118</v>
       </c>
-      <c r="C58" s="21" t="s">
+      <c r="C59" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="D58" s="7">
+      <c r="D59" s="7">
         <v>4</v>
       </c>
-      <c r="E58" s="8" t="s">
+      <c r="E59" s="8" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" s="21" t="s">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" s="16" t="s">
         <v>130</v>
       </c>
-      <c r="B59" s="21" t="s">
+      <c r="B60" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="C59" s="21" t="s">
+      <c r="C60" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="D59" s="3">
-        <v>2</v>
-      </c>
-      <c r="E59" s="4" t="s">
+      <c r="D60" s="3">
+        <v>2</v>
+      </c>
+      <c r="E60" s="4" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" s="21" t="s">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" s="16" t="s">
         <v>130</v>
       </c>
-      <c r="B60" s="21" t="s">
+      <c r="B61" s="16" t="s">
         <v>120</v>
       </c>
-      <c r="C60" s="21" t="s">
+      <c r="C61" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="D60" s="5">
-        <v>1</v>
-      </c>
-      <c r="E60" s="6" t="s">
+      <c r="D61" s="5">
+        <v>1</v>
+      </c>
+      <c r="E61" s="6" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A61" s="21" t="s">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" s="16" t="s">
         <v>130</v>
       </c>
-      <c r="B61" s="21" t="s">
+      <c r="B62" s="16" t="s">
         <v>121</v>
       </c>
-      <c r="C61" s="21" t="s">
+      <c r="C62" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="D61" s="5">
-        <v>1</v>
-      </c>
-      <c r="E61" s="6" t="s">
+      <c r="D62" s="5">
+        <v>1</v>
+      </c>
+      <c r="E62" s="6" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" s="21" t="s">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" s="16" t="s">
         <v>130</v>
       </c>
-      <c r="B62" s="21" t="s">
+      <c r="B63" s="16" t="s">
         <v>122</v>
       </c>
-      <c r="C62" s="21" t="s">
+      <c r="C63" s="16" t="s">
         <v>60</v>
-      </c>
-      <c r="D62" s="7">
-        <v>4</v>
-      </c>
-      <c r="E62" s="8" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A63" s="21" t="s">
-        <v>130</v>
-      </c>
-      <c r="B63" s="21" t="s">
-        <v>123</v>
-      </c>
-      <c r="C63" s="21" t="s">
-        <v>61</v>
       </c>
       <c r="D63" s="7">
         <v>4</v>
       </c>
       <c r="E63" s="8" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="B64" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="C64" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="D64" s="7">
+        <v>4</v>
+      </c>
+      <c r="E64" s="8" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A64" s="21" t="s">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" s="16" t="s">
         <v>130</v>
       </c>
-      <c r="B64" s="21" t="s">
+      <c r="B65" s="16" t="s">
         <v>124</v>
       </c>
-      <c r="C64" s="21" t="s">
+      <c r="C65" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="D64" s="3">
-        <v>2</v>
-      </c>
-      <c r="E64" s="4" t="s">
+      <c r="D65" s="3">
+        <v>2</v>
+      </c>
+      <c r="E65" s="4" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A65" s="23" t="s">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" s="18" t="s">
         <v>130</v>
       </c>
-      <c r="B65" s="23" t="s">
+      <c r="B66" s="18" t="s">
         <v>125</v>
       </c>
-      <c r="C65" s="23" t="s">
+      <c r="C66" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="D65" s="25">
-        <v>1</v>
-      </c>
-      <c r="E65" s="26" t="s">
+      <c r="D66" s="20">
+        <v>1</v>
+      </c>
+      <c r="E66" s="21" t="s">
         <v>191</v>
       </c>
     </row>
@@ -2339,1137 +2312,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E65"/>
-  <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="88.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" style="2"/>
-    <col min="5" max="5" width="11.42578125" style="20"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="14" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>126</v>
-      </c>
-      <c r="B2" t="s">
-        <v>90</v>
-      </c>
-      <c r="C2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D2" s="5">
-        <v>1</v>
-      </c>
-      <c r="E2" s="15">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>128</v>
-      </c>
-      <c r="B3" t="s">
-        <v>103</v>
-      </c>
-      <c r="C3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D3" s="5">
-        <v>1</v>
-      </c>
-      <c r="E3" s="15">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>126</v>
-      </c>
-      <c r="B4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="5">
-        <v>1</v>
-      </c>
-      <c r="E4" s="15">
-        <v>0.04</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>128</v>
-      </c>
-      <c r="B5" t="s">
-        <v>108</v>
-      </c>
-      <c r="C5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D5" s="5">
-        <v>1</v>
-      </c>
-      <c r="E5" s="15">
-        <v>0.04</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>128</v>
-      </c>
-      <c r="B6" t="s">
-        <v>104</v>
-      </c>
-      <c r="C6" t="s">
-        <v>43</v>
-      </c>
-      <c r="D6" s="5">
-        <v>1</v>
-      </c>
-      <c r="E6" s="15">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>130</v>
-      </c>
-      <c r="B7" t="s">
-        <v>120</v>
-      </c>
-      <c r="C7" t="s">
-        <v>58</v>
-      </c>
-      <c r="D7" s="5">
-        <v>1</v>
-      </c>
-      <c r="E7" s="15">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>130</v>
-      </c>
-      <c r="B8" t="s">
-        <v>125</v>
-      </c>
-      <c r="C8" t="s">
-        <v>63</v>
-      </c>
-      <c r="D8" s="5">
-        <v>1</v>
-      </c>
-      <c r="E8" s="15">
-        <v>0.14000000000000001</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>130</v>
-      </c>
-      <c r="B9" t="s">
-        <v>121</v>
-      </c>
-      <c r="C9" t="s">
-        <v>59</v>
-      </c>
-      <c r="D9" s="5">
-        <v>1</v>
-      </c>
-      <c r="E9" s="15">
-        <v>0.16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>126</v>
-      </c>
-      <c r="B10" t="s">
-        <v>91</v>
-      </c>
-      <c r="C10" t="s">
-        <v>32</v>
-      </c>
-      <c r="D10" s="5">
-        <v>1</v>
-      </c>
-      <c r="E10" s="15">
-        <v>0.17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>128</v>
-      </c>
-      <c r="B11" t="s">
-        <v>102</v>
-      </c>
-      <c r="C11" t="s">
-        <v>41</v>
-      </c>
-      <c r="D11" s="5">
-        <v>1</v>
-      </c>
-      <c r="E11" s="15">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>126</v>
-      </c>
-      <c r="B12" t="s">
-        <v>69</v>
-      </c>
-      <c r="C12" t="s">
-        <v>9</v>
-      </c>
-      <c r="D12" s="5">
-        <v>1</v>
-      </c>
-      <c r="E12" s="15">
-        <v>0.22</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>128</v>
-      </c>
-      <c r="B13" t="s">
-        <v>107</v>
-      </c>
-      <c r="C13" t="s">
-        <v>197</v>
-      </c>
-      <c r="D13" s="5">
-        <v>1</v>
-      </c>
-      <c r="E13" s="15">
-        <v>0.24</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>127</v>
-      </c>
-      <c r="B14" t="s">
-        <v>96</v>
-      </c>
-      <c r="C14" t="s">
-        <v>35</v>
-      </c>
-      <c r="D14" s="5">
-        <v>1</v>
-      </c>
-      <c r="E14" s="15">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>126</v>
-      </c>
-      <c r="B15" t="s">
-        <v>66</v>
-      </c>
-      <c r="C15" t="s">
-        <v>6</v>
-      </c>
-      <c r="D15" s="5">
-        <v>1</v>
-      </c>
-      <c r="E15" s="15">
-        <v>0.26</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>128</v>
-      </c>
-      <c r="B16" t="s">
-        <v>97</v>
-      </c>
-      <c r="C16" t="s">
-        <v>36</v>
-      </c>
-      <c r="D16" s="5">
-        <v>1</v>
-      </c>
-      <c r="E16" s="15">
-        <v>0.28000000000000003</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>128</v>
-      </c>
-      <c r="B17" t="s">
-        <v>98</v>
-      </c>
-      <c r="C17" t="s">
-        <v>37</v>
-      </c>
-      <c r="D17" s="5">
-        <v>1</v>
-      </c>
-      <c r="E17" s="15">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>126</v>
-      </c>
-      <c r="B18" t="s">
-        <v>76</v>
-      </c>
-      <c r="C18" t="s">
-        <v>17</v>
-      </c>
-      <c r="D18" s="5">
-        <v>1</v>
-      </c>
-      <c r="E18" s="15">
-        <v>0.35</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>126</v>
-      </c>
-      <c r="B19" t="s">
-        <v>81</v>
-      </c>
-      <c r="C19" t="s">
-        <v>22</v>
-      </c>
-      <c r="D19" s="5">
-        <v>1</v>
-      </c>
-      <c r="E19" s="15">
-        <v>0.35</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>129</v>
-      </c>
-      <c r="B20" t="s">
-        <v>111</v>
-      </c>
-      <c r="C20" t="s">
-        <v>49</v>
-      </c>
-      <c r="D20" s="5">
-        <v>1</v>
-      </c>
-      <c r="E20" s="15">
-        <v>0.36</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>128</v>
-      </c>
-      <c r="B21" t="s">
-        <v>99</v>
-      </c>
-      <c r="C21" t="s">
-        <v>38</v>
-      </c>
-      <c r="D21" s="5">
-        <v>1</v>
-      </c>
-      <c r="E21" s="15">
-        <v>0.37</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>126</v>
-      </c>
-      <c r="B22" t="s">
-        <v>192</v>
-      </c>
-      <c r="C22" t="s">
-        <v>193</v>
-      </c>
-      <c r="D22" s="5">
-        <v>1</v>
-      </c>
-      <c r="E22" s="15">
-        <v>0.42</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>127</v>
-      </c>
-      <c r="B23" t="s">
-        <v>93</v>
-      </c>
-      <c r="C23" t="s">
-        <v>9</v>
-      </c>
-      <c r="D23" s="5">
-        <v>1</v>
-      </c>
-      <c r="E23" s="15">
-        <v>0.42</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>127</v>
-      </c>
-      <c r="B24" t="s">
-        <v>95</v>
-      </c>
-      <c r="C24" t="s">
-        <v>34</v>
-      </c>
-      <c r="D24" s="5">
-        <v>1</v>
-      </c>
-      <c r="E24" s="15">
-        <v>0.43</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>128</v>
-      </c>
-      <c r="B25" t="s">
-        <v>100</v>
-      </c>
-      <c r="C25" t="s">
-        <v>39</v>
-      </c>
-      <c r="D25" s="5">
-        <v>1</v>
-      </c>
-      <c r="E25" s="15">
-        <v>0.48</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>126</v>
-      </c>
-      <c r="B26" t="s">
-        <v>77</v>
-      </c>
-      <c r="C26" t="s">
-        <v>18</v>
-      </c>
-      <c r="D26" s="5">
-        <v>1</v>
-      </c>
-      <c r="E26" s="15">
-        <v>0.49</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>126</v>
-      </c>
-      <c r="B27" t="s">
-        <v>79</v>
-      </c>
-      <c r="C27" t="s">
-        <v>20</v>
-      </c>
-      <c r="D27" s="5">
-        <v>1</v>
-      </c>
-      <c r="E27" s="15">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>126</v>
-      </c>
-      <c r="B28" t="s">
-        <v>80</v>
-      </c>
-      <c r="C28" t="s">
-        <v>21</v>
-      </c>
-      <c r="D28" s="5">
-        <v>1</v>
-      </c>
-      <c r="E28" s="15">
-        <v>0.54</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>126</v>
-      </c>
-      <c r="B29" t="s">
-        <v>133</v>
-      </c>
-      <c r="C29" t="s">
-        <v>10</v>
-      </c>
-      <c r="D29" s="5">
-        <v>1</v>
-      </c>
-      <c r="E29" s="15">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>127</v>
-      </c>
-      <c r="B30" t="s">
-        <v>94</v>
-      </c>
-      <c r="C30" t="s">
-        <v>33</v>
-      </c>
-      <c r="D30" s="5">
-        <v>1</v>
-      </c>
-      <c r="E30" s="15">
-        <v>0.74</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>130</v>
-      </c>
-      <c r="B31" t="s">
-        <v>115</v>
-      </c>
-      <c r="C31" t="s">
-        <v>53</v>
-      </c>
-      <c r="D31" s="5">
-        <v>1</v>
-      </c>
-      <c r="E31" s="15">
-        <v>0.92</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>126</v>
-      </c>
-      <c r="B32" t="s">
-        <v>78</v>
-      </c>
-      <c r="C32" t="s">
-        <v>19</v>
-      </c>
-      <c r="D32" s="5">
-        <v>1</v>
-      </c>
-      <c r="E32" s="15">
-        <v>0.93</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>126</v>
-      </c>
-      <c r="B33" t="s">
-        <v>71</v>
-      </c>
-      <c r="C33" t="s">
-        <v>12</v>
-      </c>
-      <c r="D33" s="5">
-        <v>1</v>
-      </c>
-      <c r="E33" s="15">
-        <v>0.96</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>126</v>
-      </c>
-      <c r="B34" t="s">
-        <v>84</v>
-      </c>
-      <c r="C34" t="s">
-        <v>25</v>
-      </c>
-      <c r="D34" s="3">
-        <v>2</v>
-      </c>
-      <c r="E34" s="16">
-        <v>1.07</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>126</v>
-      </c>
-      <c r="B35" t="s">
-        <v>70</v>
-      </c>
-      <c r="C35" t="s">
-        <v>11</v>
-      </c>
-      <c r="D35" s="3">
-        <v>2</v>
-      </c>
-      <c r="E35" s="16">
-        <v>1.1000000000000001</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>126</v>
-      </c>
-      <c r="B36" t="s">
-        <v>85</v>
-      </c>
-      <c r="C36" t="s">
-        <v>26</v>
-      </c>
-      <c r="D36" s="3">
-        <v>2</v>
-      </c>
-      <c r="E36" s="16">
-        <v>1.1000000000000001</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>126</v>
-      </c>
-      <c r="B37" t="s">
-        <v>72</v>
-      </c>
-      <c r="C37" t="s">
-        <v>13</v>
-      </c>
-      <c r="D37" s="3">
-        <v>2</v>
-      </c>
-      <c r="E37" s="16">
-        <v>1.1100000000000001</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>126</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C38" t="s">
-        <v>4</v>
-      </c>
-      <c r="D38" s="3">
-        <v>2</v>
-      </c>
-      <c r="E38" s="16">
-        <v>1.1200000000000001</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>128</v>
-      </c>
-      <c r="B39" t="s">
-        <v>106</v>
-      </c>
-      <c r="C39" t="s">
-        <v>45</v>
-      </c>
-      <c r="D39" s="3">
-        <v>2</v>
-      </c>
-      <c r="E39" s="16">
-        <v>1.1499999999999999</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>128</v>
-      </c>
-      <c r="B40" t="s">
-        <v>101</v>
-      </c>
-      <c r="C40" t="s">
-        <v>40</v>
-      </c>
-      <c r="D40" s="3">
-        <v>2</v>
-      </c>
-      <c r="E40" s="16">
-        <v>1.21</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>126</v>
-      </c>
-      <c r="B41" t="s">
-        <v>89</v>
-      </c>
-      <c r="C41" t="s">
-        <v>30</v>
-      </c>
-      <c r="D41" s="3">
-        <v>2</v>
-      </c>
-      <c r="E41" s="16">
-        <v>1.59</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>126</v>
-      </c>
-      <c r="B42" t="s">
-        <v>88</v>
-      </c>
-      <c r="C42" t="s">
-        <v>29</v>
-      </c>
-      <c r="D42" s="3">
-        <v>2</v>
-      </c>
-      <c r="E42" s="16">
-        <v>1.62</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>128</v>
-      </c>
-      <c r="B43" t="s">
-        <v>105</v>
-      </c>
-      <c r="C43" t="s">
-        <v>44</v>
-      </c>
-      <c r="D43" s="3">
-        <v>2</v>
-      </c>
-      <c r="E43" s="16">
-        <v>1.8</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>129</v>
-      </c>
-      <c r="B44" t="s">
-        <v>109</v>
-      </c>
-      <c r="C44" t="s">
-        <v>47</v>
-      </c>
-      <c r="D44" s="3">
-        <v>2</v>
-      </c>
-      <c r="E44" s="16">
-        <v>2.14</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>130</v>
-      </c>
-      <c r="B45" t="s">
-        <v>116</v>
-      </c>
-      <c r="C45" t="s">
-        <v>54</v>
-      </c>
-      <c r="D45" s="3">
-        <v>2</v>
-      </c>
-      <c r="E45" s="16">
-        <v>2.42</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>127</v>
-      </c>
-      <c r="B46" t="s">
-        <v>92</v>
-      </c>
-      <c r="C46" t="s">
-        <v>8</v>
-      </c>
-      <c r="D46" s="3">
-        <v>2</v>
-      </c>
-      <c r="E46" s="16">
-        <v>2.64</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>126</v>
-      </c>
-      <c r="B47" t="s">
-        <v>68</v>
-      </c>
-      <c r="C47" t="s">
-        <v>8</v>
-      </c>
-      <c r="D47" s="3">
-        <v>2</v>
-      </c>
-      <c r="E47" s="16">
-        <v>2.89</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>130</v>
-      </c>
-      <c r="B48" t="s">
-        <v>117</v>
-      </c>
-      <c r="C48" t="s">
-        <v>55</v>
-      </c>
-      <c r="D48" s="3">
-        <v>2</v>
-      </c>
-      <c r="E48" s="16">
-        <v>2.92</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>129</v>
-      </c>
-      <c r="B49" t="s">
-        <v>113</v>
-      </c>
-      <c r="C49" t="s">
-        <v>51</v>
-      </c>
-      <c r="D49" s="3">
-        <v>2</v>
-      </c>
-      <c r="E49" s="16">
-        <v>3.31</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>129</v>
-      </c>
-      <c r="B50" t="s">
-        <v>112</v>
-      </c>
-      <c r="C50" t="s">
-        <v>50</v>
-      </c>
-      <c r="D50" s="3">
-        <v>2</v>
-      </c>
-      <c r="E50" s="16">
-        <v>3.5</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>126</v>
-      </c>
-      <c r="B51" t="s">
-        <v>75</v>
-      </c>
-      <c r="C51" t="s">
-        <v>16</v>
-      </c>
-      <c r="D51" s="3">
-        <v>2</v>
-      </c>
-      <c r="E51" s="16">
-        <v>3.58</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>129</v>
-      </c>
-      <c r="B52" t="s">
-        <v>110</v>
-      </c>
-      <c r="C52" t="s">
-        <v>48</v>
-      </c>
-      <c r="D52" s="3">
-        <v>2</v>
-      </c>
-      <c r="E52" s="16">
-        <v>3.69</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>130</v>
-      </c>
-      <c r="B53" t="s">
-        <v>124</v>
-      </c>
-      <c r="C53" t="s">
-        <v>62</v>
-      </c>
-      <c r="D53" s="3">
-        <v>2</v>
-      </c>
-      <c r="E53" s="16">
-        <v>3.75</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>130</v>
-      </c>
-      <c r="B54" t="s">
-        <v>119</v>
-      </c>
-      <c r="C54" t="s">
-        <v>57</v>
-      </c>
-      <c r="D54" s="3">
-        <v>2</v>
-      </c>
-      <c r="E54" s="16">
-        <v>4.45</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>129</v>
-      </c>
-      <c r="B55" t="s">
-        <v>114</v>
-      </c>
-      <c r="C55" t="s">
-        <v>52</v>
-      </c>
-      <c r="D55" s="3">
-        <v>2</v>
-      </c>
-      <c r="E55" s="16">
-        <v>4.88</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>126</v>
-      </c>
-      <c r="B56" t="s">
-        <v>67</v>
-      </c>
-      <c r="C56" t="s">
-        <v>7</v>
-      </c>
-      <c r="D56" s="11">
-        <v>3</v>
-      </c>
-      <c r="E56" s="17">
-        <v>18.350000000000001</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>130</v>
-      </c>
-      <c r="B57" t="s">
-        <v>122</v>
-      </c>
-      <c r="C57" t="s">
-        <v>60</v>
-      </c>
-      <c r="D57" s="7">
-        <v>4</v>
-      </c>
-      <c r="E57" s="18">
-        <v>29.83</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>126</v>
-      </c>
-      <c r="B58" t="s">
-        <v>73</v>
-      </c>
-      <c r="C58" t="s">
-        <v>14</v>
-      </c>
-      <c r="D58" s="7">
-        <v>4</v>
-      </c>
-      <c r="E58" s="18">
-        <v>38.409999999999997</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>130</v>
-      </c>
-      <c r="B59" t="s">
-        <v>123</v>
-      </c>
-      <c r="C59" t="s">
-        <v>61</v>
-      </c>
-      <c r="D59" s="7">
-        <v>4</v>
-      </c>
-      <c r="E59" s="18">
-        <v>39.08</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>126</v>
-      </c>
-      <c r="B60" t="s">
-        <v>86</v>
-      </c>
-      <c r="C60" t="s">
-        <v>27</v>
-      </c>
-      <c r="D60" s="7">
-        <v>4</v>
-      </c>
-      <c r="E60" s="18">
-        <v>39.880000000000003</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>126</v>
-      </c>
-      <c r="B61" t="s">
-        <v>82</v>
-      </c>
-      <c r="C61" t="s">
-        <v>23</v>
-      </c>
-      <c r="D61" s="7">
-        <v>4</v>
-      </c>
-      <c r="E61" s="18">
-        <v>45.9</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>126</v>
-      </c>
-      <c r="B62" t="s">
-        <v>83</v>
-      </c>
-      <c r="C62" t="s">
-        <v>24</v>
-      </c>
-      <c r="D62" s="7">
-        <v>4</v>
-      </c>
-      <c r="E62" s="18">
-        <v>46.31</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>126</v>
-      </c>
-      <c r="B63" t="s">
-        <v>87</v>
-      </c>
-      <c r="C63" t="s">
-        <v>28</v>
-      </c>
-      <c r="D63" s="7">
-        <v>4</v>
-      </c>
-      <c r="E63" s="18">
-        <v>47.18</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>130</v>
-      </c>
-      <c r="B64" t="s">
-        <v>118</v>
-      </c>
-      <c r="C64" t="s">
-        <v>56</v>
-      </c>
-      <c r="D64" s="7">
-        <v>4</v>
-      </c>
-      <c r="E64" s="18">
-        <v>48.43</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>126</v>
-      </c>
-      <c r="B65" t="s">
-        <v>74</v>
-      </c>
-      <c r="C65" t="s">
-        <v>15</v>
-      </c>
-      <c r="D65" s="9">
-        <v>5</v>
-      </c>
-      <c r="E65" s="19">
-        <v>168.9</v>
-      </c>
-    </row>
-  </sheetData>
-  <sortState ref="A2:E65">
-    <sortCondition ref="E2:E65"/>
-  </sortState>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F65"/>
+  <dimension ref="A1:F66"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
@@ -3480,7 +2323,7 @@
     <col min="3" max="3" width="17.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="88.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.5703125" style="20" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.5703125" style="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -3504,7 +2347,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="29">
+      <c r="A2" s="24">
         <v>1</v>
       </c>
       <c r="B2" t="s">
@@ -3519,12 +2362,12 @@
       <c r="E2" s="5">
         <v>1</v>
       </c>
-      <c r="F2" s="30" t="s">
+      <c r="F2" s="25" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="29">
+      <c r="A3" s="24">
         <v>2</v>
       </c>
       <c r="B3" t="s">
@@ -3539,12 +2382,12 @@
       <c r="E3" s="5">
         <v>1</v>
       </c>
-      <c r="F3" s="30" t="s">
+      <c r="F3" s="25" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="29">
+      <c r="A4" s="24">
         <v>3</v>
       </c>
       <c r="B4" t="s">
@@ -3559,12 +2402,12 @@
       <c r="E4" s="5">
         <v>1</v>
       </c>
-      <c r="F4" s="30" t="s">
+      <c r="F4" s="25" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="29">
+      <c r="A5" s="24">
         <v>4</v>
       </c>
       <c r="B5" t="s">
@@ -3579,12 +2422,12 @@
       <c r="E5" s="5">
         <v>1</v>
       </c>
-      <c r="F5" s="30" t="s">
+      <c r="F5" s="25" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="29">
+      <c r="A6" s="24">
         <v>5</v>
       </c>
       <c r="B6" t="s">
@@ -3599,12 +2442,12 @@
       <c r="E6" s="5">
         <v>1</v>
       </c>
-      <c r="F6" s="30" t="s">
+      <c r="F6" s="25" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="29">
+      <c r="A7" s="24">
         <v>6</v>
       </c>
       <c r="B7" t="s">
@@ -3619,12 +2462,12 @@
       <c r="E7" s="5">
         <v>1</v>
       </c>
-      <c r="F7" s="30" t="s">
+      <c r="F7" s="25" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="29">
+      <c r="A8" s="24">
         <v>7</v>
       </c>
       <c r="B8" t="s">
@@ -3639,12 +2482,12 @@
       <c r="E8" s="5">
         <v>1</v>
       </c>
-      <c r="F8" s="30" t="s">
+      <c r="F8" s="25" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="29">
+      <c r="A9" s="24">
         <v>8</v>
       </c>
       <c r="B9" t="s">
@@ -3659,12 +2502,12 @@
       <c r="E9" s="5">
         <v>1</v>
       </c>
-      <c r="F9" s="30" t="s">
+      <c r="F9" s="25" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="29">
+      <c r="A10" s="24">
         <v>9</v>
       </c>
       <c r="B10" t="s">
@@ -3679,12 +2522,12 @@
       <c r="E10" s="5">
         <v>1</v>
       </c>
-      <c r="F10" s="30" t="s">
+      <c r="F10" s="25" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="29">
+      <c r="A11" s="24">
         <v>10</v>
       </c>
       <c r="B11" t="s">
@@ -3699,12 +2542,12 @@
       <c r="E11" s="5">
         <v>1</v>
       </c>
-      <c r="F11" s="30" t="s">
+      <c r="F11" s="25" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="29">
+      <c r="A12" s="24">
         <v>11</v>
       </c>
       <c r="B12" t="s">
@@ -3719,12 +2562,12 @@
       <c r="E12" s="5">
         <v>1</v>
       </c>
-      <c r="F12" s="30" t="s">
+      <c r="F12" s="25" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="29">
+      <c r="A13" s="24">
         <v>12</v>
       </c>
       <c r="B13" t="s">
@@ -3739,12 +2582,12 @@
       <c r="E13" s="5">
         <v>1</v>
       </c>
-      <c r="F13" s="30" t="s">
+      <c r="F13" s="25" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="29">
+      <c r="A14" s="24">
         <v>13</v>
       </c>
       <c r="B14" t="s">
@@ -3759,12 +2602,12 @@
       <c r="E14" s="5">
         <v>1</v>
       </c>
-      <c r="F14" s="30" t="s">
+      <c r="F14" s="25" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="29">
+      <c r="A15" s="24">
         <v>14</v>
       </c>
       <c r="B15" t="s">
@@ -3779,12 +2622,12 @@
       <c r="E15" s="5">
         <v>1</v>
       </c>
-      <c r="F15" s="30" t="s">
+      <c r="F15" s="25" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="29">
+      <c r="A16" s="24">
         <v>15</v>
       </c>
       <c r="B16" t="s">
@@ -3799,12 +2642,12 @@
       <c r="E16" s="5">
         <v>1</v>
       </c>
-      <c r="F16" s="30" t="s">
+      <c r="F16" s="25" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="29">
+      <c r="A17" s="24">
         <v>16</v>
       </c>
       <c r="B17" t="s">
@@ -3819,12 +2662,12 @@
       <c r="E17" s="5">
         <v>1</v>
       </c>
-      <c r="F17" s="30" t="s">
+      <c r="F17" s="25" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="29">
+      <c r="A18" s="24">
         <v>17</v>
       </c>
       <c r="B18" t="s">
@@ -3839,12 +2682,12 @@
       <c r="E18" s="5">
         <v>1</v>
       </c>
-      <c r="F18" s="30" t="s">
+      <c r="F18" s="25" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="29">
+      <c r="A19" s="24">
         <v>18</v>
       </c>
       <c r="B19" t="s">
@@ -3859,12 +2702,12 @@
       <c r="E19" s="5">
         <v>1</v>
       </c>
-      <c r="F19" s="30" t="s">
+      <c r="F19" s="25" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="29">
+      <c r="A20" s="24">
         <v>19</v>
       </c>
       <c r="B20" t="s">
@@ -3879,12 +2722,12 @@
       <c r="E20" s="5">
         <v>1</v>
       </c>
-      <c r="F20" s="30" t="s">
+      <c r="F20" s="25" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="29">
+      <c r="A21" s="24">
         <v>20</v>
       </c>
       <c r="B21" t="s">
@@ -3899,12 +2742,12 @@
       <c r="E21" s="5">
         <v>1</v>
       </c>
-      <c r="F21" s="30" t="s">
+      <c r="F21" s="25" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="29">
+      <c r="A22" s="24">
         <v>21</v>
       </c>
       <c r="B22" t="s">
@@ -3919,12 +2762,12 @@
       <c r="E22" s="5">
         <v>1</v>
       </c>
-      <c r="F22" s="30" t="s">
+      <c r="F22" s="25" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="29">
+      <c r="A23" s="24">
         <v>22</v>
       </c>
       <c r="B23" t="s">
@@ -3939,12 +2782,12 @@
       <c r="E23" s="5">
         <v>1</v>
       </c>
-      <c r="F23" s="30" t="s">
+      <c r="F23" s="25" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="29">
+      <c r="A24" s="24">
         <v>23</v>
       </c>
       <c r="B24" t="s">
@@ -3959,12 +2802,12 @@
       <c r="E24" s="5">
         <v>1</v>
       </c>
-      <c r="F24" s="30" t="s">
+      <c r="F24" s="25" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="29">
+      <c r="A25" s="24">
         <v>24</v>
       </c>
       <c r="B25" t="s">
@@ -3979,12 +2822,12 @@
       <c r="E25" s="5">
         <v>1</v>
       </c>
-      <c r="F25" s="30" t="s">
+      <c r="F25" s="25" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="29">
+      <c r="A26" s="24">
         <v>25</v>
       </c>
       <c r="B26" t="s">
@@ -3999,12 +2842,12 @@
       <c r="E26" s="5">
         <v>1</v>
       </c>
-      <c r="F26" s="30" t="s">
+      <c r="F26" s="25" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="29">
+      <c r="A27" s="24">
         <v>26</v>
       </c>
       <c r="B27" t="s">
@@ -4019,12 +2862,12 @@
       <c r="E27" s="5">
         <v>1</v>
       </c>
-      <c r="F27" s="30" t="s">
+      <c r="F27" s="25" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="29">
+      <c r="A28" s="24">
         <v>27</v>
       </c>
       <c r="B28" t="s">
@@ -4039,12 +2882,12 @@
       <c r="E28" s="5">
         <v>1</v>
       </c>
-      <c r="F28" s="30" t="s">
+      <c r="F28" s="25" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="29">
+      <c r="A29" s="24">
         <v>28</v>
       </c>
       <c r="B29" t="s">
@@ -4059,12 +2902,12 @@
       <c r="E29" s="5">
         <v>1</v>
       </c>
-      <c r="F29" s="30" t="s">
+      <c r="F29" s="25" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="29">
+      <c r="A30" s="24">
         <v>29</v>
       </c>
       <c r="B30" t="s">
@@ -4079,12 +2922,12 @@
       <c r="E30" s="5">
         <v>1</v>
       </c>
-      <c r="F30" s="30" t="s">
+      <c r="F30" s="25" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="29">
+      <c r="A31" s="24">
         <v>30</v>
       </c>
       <c r="B31" t="s">
@@ -4099,12 +2942,12 @@
       <c r="E31" s="5">
         <v>1</v>
       </c>
-      <c r="F31" s="30" t="s">
+      <c r="F31" s="25" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="29">
+      <c r="A32" s="24">
         <v>31</v>
       </c>
       <c r="B32" t="s">
@@ -4119,12 +2962,12 @@
       <c r="E32" s="5">
         <v>1</v>
       </c>
-      <c r="F32" s="30" t="s">
+      <c r="F32" s="25" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="29">
+      <c r="A33" s="24">
         <v>32</v>
       </c>
       <c r="B33" t="s">
@@ -4139,12 +2982,12 @@
       <c r="E33" s="5">
         <v>1</v>
       </c>
-      <c r="F33" s="30" t="s">
+      <c r="F33" s="25" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="29">
+      <c r="A34" s="24">
         <v>33</v>
       </c>
       <c r="B34" t="s">
@@ -4159,12 +3002,12 @@
       <c r="E34" s="3">
         <v>2</v>
       </c>
-      <c r="F34" s="31" t="s">
+      <c r="F34" s="26" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="29">
+      <c r="A35" s="24">
         <v>34</v>
       </c>
       <c r="B35" t="s">
@@ -4179,12 +3022,12 @@
       <c r="E35" s="3">
         <v>2</v>
       </c>
-      <c r="F35" s="31" t="s">
+      <c r="F35" s="26" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="29">
+      <c r="A36" s="24">
         <v>35</v>
       </c>
       <c r="B36" t="s">
@@ -4199,12 +3042,12 @@
       <c r="E36" s="3">
         <v>2</v>
       </c>
-      <c r="F36" s="31" t="s">
+      <c r="F36" s="26" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="29">
+      <c r="A37" s="24">
         <v>36</v>
       </c>
       <c r="B37" t="s">
@@ -4219,12 +3062,12 @@
       <c r="E37" s="3">
         <v>2</v>
       </c>
-      <c r="F37" s="31" t="s">
+      <c r="F37" s="26" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="29">
+      <c r="A38" s="24">
         <v>37</v>
       </c>
       <c r="B38" t="s">
@@ -4239,12 +3082,12 @@
       <c r="E38" s="3">
         <v>2</v>
       </c>
-      <c r="F38" s="31" t="s">
+      <c r="F38" s="26" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="29">
+      <c r="A39" s="24">
         <v>38</v>
       </c>
       <c r="B39" t="s">
@@ -4259,12 +3102,12 @@
       <c r="E39" s="3">
         <v>2</v>
       </c>
-      <c r="F39" s="31" t="s">
+      <c r="F39" s="26" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="29">
+      <c r="A40" s="24">
         <v>39</v>
       </c>
       <c r="B40" t="s">
@@ -4279,12 +3122,12 @@
       <c r="E40" s="3">
         <v>2</v>
       </c>
-      <c r="F40" s="31" t="s">
+      <c r="F40" s="26" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="29">
+      <c r="A41" s="24">
         <v>40</v>
       </c>
       <c r="B41" t="s">
@@ -4299,12 +3142,12 @@
       <c r="E41" s="3">
         <v>2</v>
       </c>
-      <c r="F41" s="31" t="s">
+      <c r="F41" s="26" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="29">
+      <c r="A42" s="24">
         <v>41</v>
       </c>
       <c r="B42" t="s">
@@ -4319,12 +3162,12 @@
       <c r="E42" s="3">
         <v>2</v>
       </c>
-      <c r="F42" s="31" t="s">
+      <c r="F42" s="26" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="29">
+      <c r="A43" s="24">
         <v>42</v>
       </c>
       <c r="B43" t="s">
@@ -4339,12 +3182,12 @@
       <c r="E43" s="3">
         <v>2</v>
       </c>
-      <c r="F43" s="31" t="s">
+      <c r="F43" s="26" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="29">
+      <c r="A44" s="24">
         <v>43</v>
       </c>
       <c r="B44" t="s">
@@ -4359,12 +3202,12 @@
       <c r="E44" s="3">
         <v>2</v>
       </c>
-      <c r="F44" s="31" t="s">
+      <c r="F44" s="26" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="29">
+      <c r="A45" s="24">
         <v>44</v>
       </c>
       <c r="B45" t="s">
@@ -4379,12 +3222,12 @@
       <c r="E45" s="3">
         <v>2</v>
       </c>
-      <c r="F45" s="31" t="s">
+      <c r="F45" s="26" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="29">
+      <c r="A46" s="24">
         <v>45</v>
       </c>
       <c r="B46" t="s">
@@ -4399,12 +3242,12 @@
       <c r="E46" s="3">
         <v>2</v>
       </c>
-      <c r="F46" s="31" t="s">
+      <c r="F46" s="26" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="29">
+      <c r="A47" s="24">
         <v>46</v>
       </c>
       <c r="B47" t="s">
@@ -4419,12 +3262,12 @@
       <c r="E47" s="3">
         <v>2</v>
       </c>
-      <c r="F47" s="31" t="s">
+      <c r="F47" s="26" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="29">
+      <c r="A48" s="24">
         <v>47</v>
       </c>
       <c r="B48" t="s">
@@ -4439,12 +3282,12 @@
       <c r="E48" s="3">
         <v>2</v>
       </c>
-      <c r="F48" s="31" t="s">
+      <c r="F48" s="26" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="29">
+      <c r="A49" s="24">
         <v>48</v>
       </c>
       <c r="B49" t="s">
@@ -4459,12 +3302,12 @@
       <c r="E49" s="3">
         <v>2</v>
       </c>
-      <c r="F49" s="31" t="s">
+      <c r="F49" s="26" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="29">
+      <c r="A50" s="24">
         <v>49</v>
       </c>
       <c r="B50" t="s">
@@ -4479,12 +3322,12 @@
       <c r="E50" s="3">
         <v>2</v>
       </c>
-      <c r="F50" s="31" t="s">
+      <c r="F50" s="26" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="29">
+      <c r="A51" s="24">
         <v>50</v>
       </c>
       <c r="B51" t="s">
@@ -4499,12 +3342,12 @@
       <c r="E51" s="3">
         <v>2</v>
       </c>
-      <c r="F51" s="31" t="s">
+      <c r="F51" s="26" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="29">
+      <c r="A52" s="24">
         <v>51</v>
       </c>
       <c r="B52" t="s">
@@ -4519,12 +3362,12 @@
       <c r="E52" s="3">
         <v>2</v>
       </c>
-      <c r="F52" s="31" t="s">
+      <c r="F52" s="26" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="29">
+      <c r="A53" s="24">
         <v>52</v>
       </c>
       <c r="B53" t="s">
@@ -4539,12 +3382,12 @@
       <c r="E53" s="3">
         <v>2</v>
       </c>
-      <c r="F53" s="31" t="s">
+      <c r="F53" s="26" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="29">
+      <c r="A54" s="24">
         <v>53</v>
       </c>
       <c r="B54" t="s">
@@ -4559,12 +3402,12 @@
       <c r="E54" s="3">
         <v>2</v>
       </c>
-      <c r="F54" s="31" t="s">
+      <c r="F54" s="26" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="29">
+      <c r="A55" s="24">
         <v>54</v>
       </c>
       <c r="B55" t="s">
@@ -4579,207 +3422,227 @@
       <c r="E55" s="3">
         <v>2</v>
       </c>
-      <c r="F55" s="31" t="s">
+      <c r="F55" s="26" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="29">
+      <c r="A56" s="24">
         <v>55</v>
       </c>
-      <c r="B56" t="s">
-        <v>126</v>
-      </c>
-      <c r="C56" t="s">
-        <v>67</v>
-      </c>
-      <c r="D56" t="s">
-        <v>7</v>
+      <c r="B56" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="C56" s="16" t="s">
+        <v>198</v>
+      </c>
+      <c r="D56" s="16" t="s">
+        <v>199</v>
       </c>
       <c r="E56" s="11">
         <v>3</v>
       </c>
-      <c r="F56" s="32" t="s">
+      <c r="F56" s="11" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" s="24">
+        <v>56</v>
+      </c>
+      <c r="B57" t="s">
+        <v>126</v>
+      </c>
+      <c r="C57" t="s">
+        <v>67</v>
+      </c>
+      <c r="D57" t="s">
+        <v>7</v>
+      </c>
+      <c r="E57" s="11">
+        <v>3</v>
+      </c>
+      <c r="F57" s="27" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="29">
-        <v>56</v>
-      </c>
-      <c r="B57" t="s">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" s="24">
+        <v>57</v>
+      </c>
+      <c r="B58" t="s">
         <v>130</v>
       </c>
-      <c r="C57" t="s">
+      <c r="C58" t="s">
         <v>122</v>
       </c>
-      <c r="D57" t="s">
+      <c r="D58" t="s">
         <v>60</v>
-      </c>
-      <c r="E57" s="7">
-        <v>4</v>
-      </c>
-      <c r="F57" s="33" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="29">
-        <v>57</v>
-      </c>
-      <c r="B58" t="s">
-        <v>126</v>
-      </c>
-      <c r="C58" t="s">
-        <v>73</v>
-      </c>
-      <c r="D58" t="s">
-        <v>14</v>
       </c>
       <c r="E58" s="7">
         <v>4</v>
       </c>
-      <c r="F58" s="33" t="s">
-        <v>146</v>
+      <c r="F58" s="28" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="29">
+      <c r="A59" s="24">
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C59" t="s">
-        <v>123</v>
+        <v>73</v>
       </c>
       <c r="D59" t="s">
-        <v>61</v>
+        <v>14</v>
       </c>
       <c r="E59" s="7">
         <v>4</v>
       </c>
-      <c r="F59" s="33" t="s">
-        <v>189</v>
+      <c r="F59" s="28" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="29">
+      <c r="A60" s="24">
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="C60" t="s">
-        <v>86</v>
+        <v>123</v>
       </c>
       <c r="D60" t="s">
-        <v>27</v>
+        <v>61</v>
       </c>
       <c r="E60" s="7">
         <v>4</v>
       </c>
-      <c r="F60" s="33" t="s">
-        <v>156</v>
+      <c r="F60" s="28" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="29">
+      <c r="A61" s="24">
         <v>60</v>
       </c>
       <c r="B61" t="s">
         <v>126</v>
       </c>
       <c r="C61" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D61" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="E61" s="7">
         <v>4</v>
       </c>
-      <c r="F61" s="33" t="s">
-        <v>152</v>
+      <c r="F61" s="28" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="29">
+      <c r="A62" s="24">
         <v>61</v>
       </c>
       <c r="B62" t="s">
         <v>126</v>
       </c>
       <c r="C62" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D62" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E62" s="7">
         <v>4</v>
       </c>
-      <c r="F62" s="33" t="s">
-        <v>153</v>
+      <c r="F62" s="28" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="29">
+      <c r="A63" s="24">
         <v>62</v>
       </c>
       <c r="B63" t="s">
         <v>126</v>
       </c>
       <c r="C63" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D63" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E63" s="7">
         <v>4</v>
       </c>
-      <c r="F63" s="33" t="s">
-        <v>157</v>
+      <c r="F63" s="28" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" s="29">
+      <c r="A64" s="24">
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C64" t="s">
-        <v>118</v>
+        <v>87</v>
       </c>
       <c r="D64" t="s">
-        <v>56</v>
+        <v>28</v>
       </c>
       <c r="E64" s="7">
         <v>4</v>
       </c>
-      <c r="F64" s="33" t="s">
+      <c r="F64" s="28" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" s="24">
+        <v>64</v>
+      </c>
+      <c r="B65" t="s">
+        <v>130</v>
+      </c>
+      <c r="C65" t="s">
+        <v>118</v>
+      </c>
+      <c r="D65" t="s">
+        <v>56</v>
+      </c>
+      <c r="E65" s="7">
+        <v>4</v>
+      </c>
+      <c r="F65" s="28" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65" s="29">
-        <v>64</v>
-      </c>
-      <c r="B65" t="s">
-        <v>126</v>
-      </c>
-      <c r="C65" t="s">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" s="24">
+        <v>65</v>
+      </c>
+      <c r="B66" t="s">
+        <v>126</v>
+      </c>
+      <c r="C66" t="s">
         <v>74</v>
       </c>
-      <c r="D65" t="s">
+      <c r="D66" t="s">
         <v>15</v>
       </c>
-      <c r="E65" s="9">
+      <c r="E66" s="9">
         <v>5</v>
       </c>
-      <c r="F65" s="34" t="s">
+      <c r="F66" s="29" t="s">
         <v>147</v>
       </c>
     </row>

</xml_diff>